<commit_message>
feat: add achievement gating to dark room demo
</commit_message>
<xml_diff>
--- a/example/game_03_a_dark_room/buildings.xlsx
+++ b/example/game_03_a_dark_room/buildings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC9"/>
+  <dimension ref="A1:CK9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,123 +449,225 @@
         <v/>
       </c>
       <c r="P1" t="str">
+        <v>Cost Scaling</v>
+      </c>
+      <c r="Q1" t="str">
         <v>Effects</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>Effect 1</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>Effect 1 Type</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>Effect 1 Resource</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>Effect 1 Amount</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
+        <v>Effect 1 Building</v>
+      </c>
+      <c r="W1" t="str">
         <v>Effect 1 Job</v>
       </c>
-      <c r="V1" t="str">
+      <c r="X1" t="str">
         <v>Effect 1 Action</v>
       </c>
-      <c r="W1" t="str">
+      <c r="Y1" t="str">
         <v>Effect 1 Event</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Z1" t="str">
         <v>Effect 1 Message</v>
       </c>
-      <c r="Y1" t="str">
-        <v/>
-      </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
+        <v/>
+      </c>
+      <c r="AB1" t="str">
         <v>Effect 2</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AC1" t="str">
         <v>Effect 2 Type</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AD1" t="str">
         <v>Effect 2 Resource</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="AE1" t="str">
         <v>Effect 2 Amount</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="AF1" t="str">
+        <v>Effect 2 Building</v>
+      </c>
+      <c r="AG1" t="str">
         <v>Effect 2 Job</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AH1" t="str">
         <v>Effect 2 Action</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="AI1" t="str">
         <v>Effect 2 Event</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="AJ1" t="str">
         <v>Effect 2 Message</v>
       </c>
-      <c r="AH1" t="str">
-        <v/>
-      </c>
-      <c r="AI1" t="str">
+      <c r="AK1" t="str">
+        <v/>
+      </c>
+      <c r="AL1" t="str">
         <v>Effect 3</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="AM1" t="str">
         <v>Effect 3 Type</v>
       </c>
-      <c r="AK1" t="str">
+      <c r="AN1" t="str">
         <v>Effect 3 Resource</v>
       </c>
-      <c r="AL1" t="str">
+      <c r="AO1" t="str">
         <v>Effect 3 Amount</v>
       </c>
-      <c r="AM1" t="str">
+      <c r="AP1" t="str">
+        <v>Effect 3 Building</v>
+      </c>
+      <c r="AQ1" t="str">
         <v>Effect 3 Job</v>
       </c>
-      <c r="AN1" t="str">
+      <c r="AR1" t="str">
         <v>Effect 3 Action</v>
       </c>
-      <c r="AO1" t="str">
+      <c r="AS1" t="str">
         <v>Effect 3 Event</v>
       </c>
-      <c r="AP1" t="str">
+      <c r="AT1" t="str">
         <v>Effect 3 Message</v>
       </c>
-      <c r="AQ1" t="str">
-        <v/>
-      </c>
-      <c r="AR1" t="str">
-        <v/>
-      </c>
-      <c r="AS1" t="str">
+      <c r="AU1" t="str">
+        <v/>
+      </c>
+      <c r="AV1" t="str">
+        <v>Effect 4</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>Effect 4 Type</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>Effect 4 Resource</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Effect 4 Amount</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Effect 4 Building</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Effect 4 Job</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>Effect 4 Action</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>Effect 4 Event</v>
+      </c>
+      <c r="BD1" t="str">
+        <v>Effect 4 Message</v>
+      </c>
+      <c r="BE1" t="str">
+        <v/>
+      </c>
+      <c r="BF1" t="str">
+        <v>Effect 5</v>
+      </c>
+      <c r="BG1" t="str">
+        <v>Effect 5 Type</v>
+      </c>
+      <c r="BH1" t="str">
+        <v>Effect 5 Resource</v>
+      </c>
+      <c r="BI1" t="str">
+        <v>Effect 5 Amount</v>
+      </c>
+      <c r="BJ1" t="str">
+        <v>Effect 5 Building</v>
+      </c>
+      <c r="BK1" t="str">
+        <v>Effect 5 Job</v>
+      </c>
+      <c r="BL1" t="str">
+        <v>Effect 5 Action</v>
+      </c>
+      <c r="BM1" t="str">
+        <v>Effect 5 Event</v>
+      </c>
+      <c r="BN1" t="str">
+        <v>Effect 5 Message</v>
+      </c>
+      <c r="BO1" t="str">
+        <v/>
+      </c>
+      <c r="BP1" t="str">
+        <v>Effect 6</v>
+      </c>
+      <c r="BQ1" t="str">
+        <v>Effect 6 Type</v>
+      </c>
+      <c r="BR1" t="str">
+        <v>Effect 6 Resource</v>
+      </c>
+      <c r="BS1" t="str">
+        <v>Effect 6 Amount</v>
+      </c>
+      <c r="BT1" t="str">
+        <v>Effect 6 Building</v>
+      </c>
+      <c r="BU1" t="str">
+        <v>Effect 6 Job</v>
+      </c>
+      <c r="BV1" t="str">
+        <v>Effect 6 Action</v>
+      </c>
+      <c r="BW1" t="str">
+        <v>Effect 6 Event</v>
+      </c>
+      <c r="BX1" t="str">
+        <v>Effect 6 Message</v>
+      </c>
+      <c r="BY1" t="str">
+        <v/>
+      </c>
+      <c r="BZ1" t="str">
+        <v/>
+      </c>
+      <c r="CA1" t="str">
         <v>Unlock</v>
       </c>
-      <c r="AT1" t="str">
+      <c r="CB1" t="str">
         <v>Unlock Building</v>
       </c>
-      <c r="AU1" t="str">
+      <c r="CC1" t="str">
         <v>Unlock Resource</v>
       </c>
-      <c r="AV1" t="str">
+      <c r="CD1" t="str">
         <v>Unlock Min</v>
       </c>
-      <c r="AW1" t="str">
+      <c r="CE1" t="str">
         <v>Unlock Max</v>
       </c>
-      <c r="AX1" t="str">
+      <c r="CF1" t="str">
         <v>Unlock Villagers</v>
       </c>
-      <c r="AY1" t="str">
+      <c r="CG1" t="str">
         <v>Unlock Event</v>
       </c>
-      <c r="AZ1" t="str">
-        <v/>
-      </c>
-      <c r="BA1" t="str">
+      <c r="CH1" t="str">
+        <v/>
+      </c>
+      <c r="CI1" t="str">
         <v>Build Time</v>
       </c>
-      <c r="BB1" t="str">
+      <c r="CJ1" t="str">
         <v>Repeatable</v>
       </c>
-      <c r="BC1" t="str">
+      <c r="CK1" t="str">
         <v>Max Count</v>
       </c>
     </row>
@@ -616,22 +718,22 @@
         <v>}</v>
       </c>
       <c r="P2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="Q2" t="str">
         <v>[</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <v>$ghost {</v>
       </c>
-      <c r="R2" t="str">
-        <v>string?</v>
-      </c>
       <c r="S2" t="str">
         <v>string?</v>
       </c>
       <c r="T2" t="str">
-        <v>float?</v>
+        <v>string?</v>
       </c>
       <c r="U2" t="str">
-        <v>uint?</v>
+        <v>float?</v>
       </c>
       <c r="V2" t="str">
         <v>uint?</v>
@@ -640,99 +742,201 @@
         <v>uint?</v>
       </c>
       <c r="X2" t="str">
-        <v>string?</v>
+        <v>uint?</v>
       </c>
       <c r="Y2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="Z2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="AA2" t="str">
         <v>}</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AB2" t="str">
         <v>$ghost {</v>
       </c>
-      <c r="AA2" t="str">
-        <v>string?</v>
-      </c>
-      <c r="AB2" t="str">
-        <v>string?</v>
-      </c>
       <c r="AC2" t="str">
-        <v>float?</v>
+        <v>string?</v>
       </c>
       <c r="AD2" t="str">
-        <v>uint?</v>
+        <v>string?</v>
       </c>
       <c r="AE2" t="str">
-        <v>uint?</v>
+        <v>float?</v>
       </c>
       <c r="AF2" t="str">
         <v>uint?</v>
       </c>
       <c r="AG2" t="str">
-        <v>string?</v>
+        <v>uint?</v>
       </c>
       <c r="AH2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="AI2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="AJ2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="AK2" t="str">
         <v>}</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AL2" t="str">
         <v>$ghost {</v>
       </c>
-      <c r="AJ2" t="str">
-        <v>string?</v>
-      </c>
-      <c r="AK2" t="str">
-        <v>string?</v>
-      </c>
-      <c r="AL2" t="str">
-        <v>float?</v>
-      </c>
       <c r="AM2" t="str">
-        <v>uint?</v>
+        <v>string?</v>
       </c>
       <c r="AN2" t="str">
-        <v>uint?</v>
+        <v>string?</v>
       </c>
       <c r="AO2" t="str">
-        <v>uint?</v>
+        <v>float?</v>
       </c>
       <c r="AP2" t="str">
-        <v>string?</v>
+        <v>uint?</v>
       </c>
       <c r="AQ2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="AR2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="AS2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="AT2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="AU2" t="str">
         <v>}</v>
       </c>
-      <c r="AR2" t="str">
+      <c r="AV2" t="str">
+        <v>$ghost {</v>
+      </c>
+      <c r="AW2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="AX2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="AY2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="AZ2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BA2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BB2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BC2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BD2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BE2" t="str">
+        <v>}</v>
+      </c>
+      <c r="BF2" t="str">
+        <v>$ghost {</v>
+      </c>
+      <c r="BG2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BH2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BI2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="BJ2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BK2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BL2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BM2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BN2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BO2" t="str">
+        <v>}</v>
+      </c>
+      <c r="BP2" t="str">
+        <v>$ghost {</v>
+      </c>
+      <c r="BQ2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BR2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BS2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="BT2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BU2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BV2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BW2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="BX2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="BY2" t="str">
+        <v>}</v>
+      </c>
+      <c r="BZ2" t="str">
         <v>]</v>
       </c>
-      <c r="AS2" t="str">
+      <c r="CA2" t="str">
         <v>{</v>
       </c>
-      <c r="AT2" t="str">
-        <v>uint?</v>
-      </c>
-      <c r="AU2" t="str">
-        <v>string?</v>
-      </c>
-      <c r="AV2" t="str">
-        <v>float?</v>
-      </c>
-      <c r="AW2" t="str">
-        <v>float?</v>
-      </c>
-      <c r="AX2" t="str">
-        <v>uint?</v>
-      </c>
-      <c r="AY2" t="str">
-        <v>uint?</v>
-      </c>
-      <c r="AZ2" t="str">
+      <c r="CB2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="CC2" t="str">
+        <v>string?</v>
+      </c>
+      <c r="CD2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="CE2" t="str">
+        <v>float?</v>
+      </c>
+      <c r="CF2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="CG2" t="str">
+        <v>uint?</v>
+      </c>
+      <c r="CH2" t="str">
         <v>}</v>
       </c>
-      <c r="BA2" t="str">
+      <c r="CI2" t="str">
         <v>float</v>
       </c>
-      <c r="BB2" t="str">
+      <c r="CJ2" t="str">
         <v>bool</v>
       </c>
-      <c r="BC2" t="str">
+      <c r="CK2" t="str">
         <v>uint</v>
       </c>
     </row>
@@ -783,123 +987,225 @@
         <v/>
       </c>
       <c r="P3" t="str">
+        <v>costScaling</v>
+      </c>
+      <c r="Q3" t="str">
         <v>effects</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <v>effect1</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <v>type</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <v>resource</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <v>amount</v>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
+        <v>building</v>
+      </c>
+      <c r="W3" t="str">
         <v>job</v>
       </c>
-      <c r="V3" t="str">
+      <c r="X3" t="str">
         <v>action</v>
       </c>
-      <c r="W3" t="str">
+      <c r="Y3" t="str">
         <v>event</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Z3" t="str">
         <v>message</v>
       </c>
-      <c r="Y3" t="str">
-        <v/>
-      </c>
-      <c r="Z3" t="str">
+      <c r="AA3" t="str">
+        <v/>
+      </c>
+      <c r="AB3" t="str">
         <v>effect2</v>
       </c>
-      <c r="AA3" t="str">
+      <c r="AC3" t="str">
         <v>type</v>
       </c>
-      <c r="AB3" t="str">
+      <c r="AD3" t="str">
         <v>resource</v>
       </c>
-      <c r="AC3" t="str">
+      <c r="AE3" t="str">
         <v>amount</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AF3" t="str">
+        <v>building</v>
+      </c>
+      <c r="AG3" t="str">
         <v>job</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AH3" t="str">
         <v>action</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AI3" t="str">
         <v>event</v>
       </c>
-      <c r="AG3" t="str">
+      <c r="AJ3" t="str">
         <v>message</v>
       </c>
-      <c r="AH3" t="str">
-        <v/>
-      </c>
-      <c r="AI3" t="str">
+      <c r="AK3" t="str">
+        <v/>
+      </c>
+      <c r="AL3" t="str">
         <v>effect3</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AM3" t="str">
         <v>type</v>
       </c>
-      <c r="AK3" t="str">
+      <c r="AN3" t="str">
         <v>resource</v>
       </c>
-      <c r="AL3" t="str">
+      <c r="AO3" t="str">
         <v>amount</v>
       </c>
-      <c r="AM3" t="str">
+      <c r="AP3" t="str">
+        <v>building</v>
+      </c>
+      <c r="AQ3" t="str">
         <v>job</v>
       </c>
-      <c r="AN3" t="str">
+      <c r="AR3" t="str">
         <v>action</v>
       </c>
-      <c r="AO3" t="str">
+      <c r="AS3" t="str">
         <v>event</v>
       </c>
-      <c r="AP3" t="str">
+      <c r="AT3" t="str">
         <v>message</v>
       </c>
-      <c r="AQ3" t="str">
-        <v/>
-      </c>
-      <c r="AR3" t="str">
-        <v/>
-      </c>
-      <c r="AS3" t="str">
+      <c r="AU3" t="str">
+        <v/>
+      </c>
+      <c r="AV3" t="str">
+        <v>effect4</v>
+      </c>
+      <c r="AW3" t="str">
+        <v>type</v>
+      </c>
+      <c r="AX3" t="str">
+        <v>resource</v>
+      </c>
+      <c r="AY3" t="str">
+        <v>amount</v>
+      </c>
+      <c r="AZ3" t="str">
+        <v>building</v>
+      </c>
+      <c r="BA3" t="str">
+        <v>job</v>
+      </c>
+      <c r="BB3" t="str">
+        <v>action</v>
+      </c>
+      <c r="BC3" t="str">
+        <v>event</v>
+      </c>
+      <c r="BD3" t="str">
+        <v>message</v>
+      </c>
+      <c r="BE3" t="str">
+        <v/>
+      </c>
+      <c r="BF3" t="str">
+        <v>effect5</v>
+      </c>
+      <c r="BG3" t="str">
+        <v>type</v>
+      </c>
+      <c r="BH3" t="str">
+        <v>resource</v>
+      </c>
+      <c r="BI3" t="str">
+        <v>amount</v>
+      </c>
+      <c r="BJ3" t="str">
+        <v>building</v>
+      </c>
+      <c r="BK3" t="str">
+        <v>job</v>
+      </c>
+      <c r="BL3" t="str">
+        <v>action</v>
+      </c>
+      <c r="BM3" t="str">
+        <v>event</v>
+      </c>
+      <c r="BN3" t="str">
+        <v>message</v>
+      </c>
+      <c r="BO3" t="str">
+        <v/>
+      </c>
+      <c r="BP3" t="str">
+        <v>effect6</v>
+      </c>
+      <c r="BQ3" t="str">
+        <v>type</v>
+      </c>
+      <c r="BR3" t="str">
+        <v>resource</v>
+      </c>
+      <c r="BS3" t="str">
+        <v>amount</v>
+      </c>
+      <c r="BT3" t="str">
+        <v>building</v>
+      </c>
+      <c r="BU3" t="str">
+        <v>job</v>
+      </c>
+      <c r="BV3" t="str">
+        <v>action</v>
+      </c>
+      <c r="BW3" t="str">
+        <v>event</v>
+      </c>
+      <c r="BX3" t="str">
+        <v>message</v>
+      </c>
+      <c r="BY3" t="str">
+        <v/>
+      </c>
+      <c r="BZ3" t="str">
+        <v/>
+      </c>
+      <c r="CA3" t="str">
         <v>unlock</v>
       </c>
-      <c r="AT3" t="str">
+      <c r="CB3" t="str">
         <v>building</v>
       </c>
-      <c r="AU3" t="str">
+      <c r="CC3" t="str">
         <v>resource</v>
       </c>
-      <c r="AV3" t="str">
+      <c r="CD3" t="str">
         <v>min</v>
       </c>
-      <c r="AW3" t="str">
+      <c r="CE3" t="str">
         <v>max</v>
       </c>
-      <c r="AX3" t="str">
+      <c r="CF3" t="str">
         <v>villagers</v>
       </c>
-      <c r="AY3" t="str">
+      <c r="CG3" t="str">
         <v>event</v>
       </c>
-      <c r="AZ3" t="str">
-        <v/>
-      </c>
-      <c r="BA3" t="str">
+      <c r="CH3" t="str">
+        <v/>
+      </c>
+      <c r="CI3" t="str">
         <v>buildTime</v>
       </c>
-      <c r="BB3" t="str">
+      <c r="CJ3" t="str">
         <v>repeatable</v>
       </c>
-      <c r="BC3" t="str">
+      <c r="CK3" t="str">
         <v>maxCount</v>
       </c>
     </row>
@@ -922,34 +1228,55 @@
       <c r="G4">
         <v>15</v>
       </c>
-      <c r="R4" t="str">
+      <c r="P4">
+        <v>0.28</v>
+      </c>
+      <c r="S4" t="str">
         <v>storage</v>
       </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
         <v>villagers</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>2</v>
       </c>
-      <c r="AA4" t="str">
+      <c r="AC4" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>20000001</v>
+      </c>
+      <c r="AM4" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AO4">
+        <v>0.5</v>
+      </c>
+      <c r="AQ4">
+        <v>20000003</v>
+      </c>
+      <c r="AW4" t="str">
         <v>event</v>
       </c>
-      <c r="AF4">
+      <c r="BC4">
         <v>50000002</v>
       </c>
-      <c r="AU4" t="str">
+      <c r="CC4" t="str">
         <v>warmth</v>
       </c>
-      <c r="AV4">
-        <v>40</v>
-      </c>
-      <c r="BA4">
+      <c r="CD4">
+        <v>60</v>
+      </c>
+      <c r="CI4">
         <v>18</v>
       </c>
-      <c r="BB4" t="b">
+      <c r="CJ4" t="b">
         <v>1</v>
       </c>
-      <c r="BC4">
+      <c r="CK4">
         <v>12</v>
       </c>
     </row>
@@ -969,40 +1296,55 @@
       <c r="F5">
         <v>25</v>
       </c>
-      <c r="R5" t="str">
+      <c r="P5">
+        <v>0.22</v>
+      </c>
+      <c r="S5" t="str">
         <v>storage</v>
       </c>
-      <c r="S5" t="str">
+      <c r="T5" t="str">
         <v>meat</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>20</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AC5" t="str">
         <v>storage</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AD5" t="str">
         <v>fur</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>20</v>
       </c>
-      <c r="AJ5" t="str">
+      <c r="AM5" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <v>20000002</v>
+      </c>
+      <c r="AW5" t="str">
         <v>unlockJob</v>
       </c>
-      <c r="AM5">
+      <c r="BA5">
         <v>20000002</v>
       </c>
-      <c r="AY5">
+      <c r="CB5">
+        <v>30000001</v>
+      </c>
+      <c r="CG5">
         <v>50000001</v>
       </c>
-      <c r="BA5">
+      <c r="CI5">
         <v>12</v>
       </c>
-      <c r="BB5" t="b">
+      <c r="CJ5" t="b">
         <v>1</v>
       </c>
-      <c r="BC5">
+      <c r="CK5">
         <v>16</v>
       </c>
     </row>
@@ -1028,31 +1370,43 @@
       <c r="H6">
         <v>20</v>
       </c>
-      <c r="R6" t="str">
+      <c r="P6">
+        <v>0.18</v>
+      </c>
+      <c r="S6" t="str">
         <v>storage</v>
       </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
         <v>supplies</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>60</v>
       </c>
-      <c r="AA6" t="str">
+      <c r="AC6" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>20000003</v>
+      </c>
+      <c r="AM6" t="str">
         <v>unlockAction</v>
       </c>
-      <c r="AE6">
+      <c r="AR6">
         <v>40000004</v>
       </c>
-      <c r="AT6">
+      <c r="CB6">
         <v>30000002</v>
       </c>
-      <c r="BA6">
+      <c r="CI6">
         <v>22</v>
       </c>
-      <c r="BB6" t="b">
+      <c r="CJ6" t="b">
         <v>0</v>
       </c>
-      <c r="BC6">
+      <c r="CK6">
         <v>2</v>
       </c>
     </row>
@@ -1078,34 +1432,58 @@
       <c r="I7">
         <v>8</v>
       </c>
-      <c r="R7" t="str">
+      <c r="P7">
+        <v>0.2</v>
+      </c>
+      <c r="S7" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="W7">
+        <v>20000004</v>
+      </c>
+      <c r="AC7" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AE7">
+        <v>1.5</v>
+      </c>
+      <c r="AG7">
+        <v>20000005</v>
+      </c>
+      <c r="AM7" t="str">
         <v>unlockJob</v>
       </c>
-      <c r="U7">
+      <c r="AQ7">
         <v>20000004</v>
       </c>
-      <c r="AA7" t="str">
+      <c r="AW7" t="str">
         <v>unlockJob</v>
       </c>
-      <c r="AD7">
+      <c r="BA7">
         <v>20000005</v>
       </c>
-      <c r="AJ7" t="str">
+      <c r="BG7" t="str">
         <v>unlockAction</v>
       </c>
-      <c r="AN7">
+      <c r="BL7">
         <v>40000005</v>
       </c>
-      <c r="AX7">
+      <c r="CB7">
+        <v>30000001</v>
+      </c>
+      <c r="CF7">
         <v>4</v>
       </c>
-      <c r="BA7">
+      <c r="CI7">
         <v>28</v>
       </c>
-      <c r="BB7" t="b">
+      <c r="CJ7" t="b">
         <v>0</v>
       </c>
-      <c r="BC7">
+      <c r="CK7">
         <v>2</v>
       </c>
     </row>
@@ -1131,37 +1509,49 @@
       <c r="K8">
         <v>35</v>
       </c>
-      <c r="R8" t="str">
+      <c r="P8">
+        <v>0.22</v>
+      </c>
+      <c r="S8" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="W8">
+        <v>20000006</v>
+      </c>
+      <c r="AC8" t="str">
+        <v>storage</v>
+      </c>
+      <c r="AD8" t="str">
+        <v>steel</v>
+      </c>
+      <c r="AE8">
+        <v>60</v>
+      </c>
+      <c r="AM8" t="str">
         <v>unlockJob</v>
       </c>
-      <c r="U8">
+      <c r="AQ8">
         <v>20000006</v>
       </c>
-      <c r="AA8" t="str">
-        <v>storage</v>
-      </c>
-      <c r="AB8" t="str">
-        <v>steel</v>
-      </c>
-      <c r="AC8">
-        <v>60</v>
-      </c>
-      <c r="AJ8" t="str">
+      <c r="AW8" t="str">
         <v>unlockAction</v>
       </c>
-      <c r="AN8">
+      <c r="BB8">
         <v>40000006</v>
       </c>
-      <c r="AT8">
+      <c r="CB8">
         <v>30000004</v>
       </c>
-      <c r="BA8">
+      <c r="CI8">
         <v>36</v>
       </c>
-      <c r="BB8" t="b">
+      <c r="CJ8" t="b">
         <v>0</v>
       </c>
-      <c r="BC8">
+      <c r="CK8">
         <v>2</v>
       </c>
     </row>
@@ -1187,37 +1577,61 @@
       <c r="L9">
         <v>10</v>
       </c>
-      <c r="R9" t="str">
+      <c r="P9">
+        <v>0.18</v>
+      </c>
+      <c r="S9" t="str">
+        <v>storage</v>
+      </c>
+      <c r="T9" t="str">
+        <v>supplies</v>
+      </c>
+      <c r="U9">
+        <v>120</v>
+      </c>
+      <c r="AC9" t="str">
+        <v>jobCap</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>20000003</v>
+      </c>
+      <c r="AM9" t="str">
         <v>unlockAction</v>
       </c>
-      <c r="V9">
+      <c r="AR9">
         <v>40000007</v>
       </c>
-      <c r="AA9" t="str">
+      <c r="AW9" t="str">
         <v>event</v>
       </c>
-      <c r="AF9">
+      <c r="BC9">
         <v>50000004</v>
       </c>
-      <c r="AU9" t="str">
+      <c r="CB9">
+        <v>30000001</v>
+      </c>
+      <c r="CC9" t="str">
         <v>supplies</v>
       </c>
-      <c r="AV9">
+      <c r="CD9">
         <v>40</v>
       </c>
-      <c r="BA9">
+      <c r="CI9">
         <v>32</v>
       </c>
-      <c r="BB9" t="b">
+      <c r="CJ9" t="b">
         <v>0</v>
       </c>
-      <c r="BC9">
+      <c r="CK9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BC9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:CK9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>